<commit_message>
fix not using batch api
</commit_message>
<xml_diff>
--- a/repos_data.xlsx
+++ b/repos_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21629\Desktop\antipattern-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE6CD8-D9E2-4488-8B31-0C2EC5C2D2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{291B4FB7-1980-4505-8831-0630F61BE758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCC6FAAD-5C78-409B-9294-FFC72811599B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B2946D8-6F95-451B-965C-A3E6FBF0F8B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>repo</t>
   </si>
   <si>
-    <t>https://github.com/gautamvr/DocumentProcessor_GCP.git</t>
-  </si>
-  <si>
-    <t>https://github.com/ovokpus/Python-Azure-AI-REST-APIs.git</t>
+    <t>https://github.com/ovokpus/Python-Azure-AI-REST-APIs</t>
   </si>
 </sst>
 </file>
@@ -426,17 +423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE7CC74-B133-4308-BDA7-BA829111A5D9}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D55BF18-2A10-4C9A-85C7-987A2A04ED52}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="49.88671875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -448,15 +442,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F19CC9E3-811C-459C-8985-70D5F22C6E71}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{9F9AD692-F1F8-4552-B7CF-52CB6CA179D1}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{102FB93A-55BA-4080-B843-C08BD25A5517}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>